<commit_message>
fairly valued...good hold, no position
</commit_message>
<xml_diff>
--- a/MCD.xlsx
+++ b/MCD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9E9C85-9F2E-0F4E-9A5C-CE8DEF35BFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6344785F-8D0F-2544-A04E-7DE596CF8723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="500" windowWidth="41500" windowHeight="23520" activeTab="1" xr2:uid="{68853114-4A9D-F642-8668-56CE329F4C0C}"/>
   </bookViews>
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBBB766-D9B8-FB40-B5C7-D36C974DF243}">
   <dimension ref="A2:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="271" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="271" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>277.8</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="3:12">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="J6" s="1">
         <f>+J4*J5</f>
-        <v>203467.2738576</v>
+        <v>201416.4878</v>
       </c>
     </row>
     <row r="7" spans="3:12">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="J9" s="1">
         <f>+J6-J7+J8</f>
-        <v>235505.17385760002</v>
+        <v>233454.38780000003</v>
       </c>
     </row>
     <row r="13" spans="3:12">
@@ -1385,10 +1385,10 @@
   <dimension ref="B2:HO114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Z6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN32" sqref="AN32"/>
+      <selection pane="bottomRight" activeCell="AW55" sqref="AW55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.1640625" defaultRowHeight="13"/>
@@ -1411,7 +1411,8 @@
     <col min="29" max="32" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="46" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="45" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="8" style="1" bestFit="1" customWidth="1"/>
@@ -2504,15 +2505,15 @@
         <v>28080.434573406877</v>
       </c>
       <c r="AL14" s="3">
-        <f t="shared" ref="AL14:AP14" si="22">+AL5*AL8/1000</f>
+        <f>+AL5*AL8/1000</f>
         <v>30454.669041509853</v>
       </c>
       <c r="AM14" s="3">
-        <f t="shared" si="22"/>
+        <f>+AM5*AM8/1000</f>
         <v>33037.185283145904</v>
       </c>
       <c r="AN14" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="AN14:AP14" si="22">+AN5*AN8/1000</f>
         <v>35846.762804676975</v>
       </c>
       <c r="AO14" s="3">
@@ -2588,11 +2589,11 @@
         <v>3153.8</v>
       </c>
       <c r="AE15" s="9">
-        <f t="shared" ref="AE15:AE29" si="24">SUM(C15:F15)</f>
+        <f t="shared" ref="AE15:AE27" si="24">SUM(C15:F15)</f>
         <v>7760.6</v>
       </c>
       <c r="AF15" s="9">
-        <f t="shared" ref="AF15:AF29" si="25">SUM(G15:J15)</f>
+        <f t="shared" ref="AF15:AF27" si="25">SUM(G15:J15)</f>
         <v>6981.2</v>
       </c>
       <c r="AG15" s="9">
@@ -5033,44 +5034,44 @@
         <v>6.6985882120643714E-2</v>
       </c>
       <c r="L36" s="49">
-        <f>+L11/H11-1</f>
+        <f t="shared" ref="L36:Q36" si="82">+L11/H11-1</f>
         <v>0.56158624584300676</v>
       </c>
       <c r="M36" s="49">
-        <f>+M11/I11-1</f>
+        <f t="shared" si="82"/>
         <v>0.13645906228131555</v>
       </c>
       <c r="N36" s="49">
-        <f>+N11/J11-1</f>
+        <f t="shared" si="82"/>
         <v>0.13679308646397703</v>
       </c>
       <c r="O36" s="49">
-        <f>+O11/K11-1</f>
+        <f t="shared" si="82"/>
         <v>6.5186213277816263E-2</v>
       </c>
       <c r="P36" s="49">
-        <f>+P11/L11-1</f>
+        <f t="shared" si="82"/>
         <v>-0.15104271306304484</v>
       </c>
       <c r="Q36" s="49">
-        <f>+Q11/M11-1</f>
+        <f t="shared" si="82"/>
         <v>-0.18226600985221675</v>
       </c>
       <c r="R36" s="39"/>
       <c r="AD36" s="49">
-        <f>+AD11/AC11-1</f>
+        <f t="shared" ref="AD36:AG37" si="83">+AD11/AC11-1</f>
         <v>-0.21276997224602745</v>
       </c>
       <c r="AE36" s="49">
-        <f>+AE11/AD11-1</f>
+        <f t="shared" si="83"/>
         <v>-5.9114924046461126E-2</v>
       </c>
       <c r="AF36" s="49">
-        <f>+AF11/AE11-1</f>
+        <f t="shared" si="83"/>
         <v>-0.13603940217391297</v>
       </c>
       <c r="AG36" s="49">
-        <f>+AG11/AF11-1</f>
+        <f t="shared" si="83"/>
         <v>0.20250147434637311</v>
       </c>
       <c r="AH36" s="42"/>
@@ -5095,64 +5096,64 @@
         <v>39</v>
       </c>
       <c r="G37" s="49">
-        <f t="shared" ref="G37:L37" si="82">+G12/C12-1</f>
+        <f t="shared" ref="G37:L37" si="84">+G12/C12-1</f>
         <v>-3.9446060918566506E-2</v>
       </c>
       <c r="H37" s="49">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-0.29001326124655724</v>
       </c>
       <c r="I37" s="49">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>1.0218978102189746E-2</v>
       </c>
       <c r="J37" s="49">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-1.3397193287989495E-4</v>
       </c>
       <c r="K37" s="49">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.10329754601227004</v>
       </c>
       <c r="L37" s="49">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.58342911877394621</v>
       </c>
       <c r="M37" s="49">
-        <f>+M12/I12-1</f>
+        <f t="shared" ref="M37:Q38" si="85">+M12/I12-1</f>
         <v>0.15285076195480807</v>
       </c>
       <c r="N37" s="49">
-        <f>+N12/J12-1</f>
+        <f t="shared" si="85"/>
         <v>0.13610022443305514</v>
       </c>
       <c r="O37" s="49">
-        <f>+O12/K12-1</f>
+        <f t="shared" si="85"/>
         <v>0.13394036282755262</v>
       </c>
       <c r="P37" s="49">
-        <f>+P12/L12-1</f>
+        <f t="shared" si="85"/>
         <v>6.6723126247655973E-2</v>
       </c>
       <c r="Q37" s="49">
-        <f>+Q12/M12-1</f>
+        <f t="shared" si="85"/>
         <v>4.5866332402712207E-2</v>
       </c>
       <c r="R37" s="39"/>
       <c r="AD37" s="49">
-        <f>+AD12/AC12-1</f>
+        <f t="shared" si="83"/>
         <v>9.0184626045636707E-2</v>
       </c>
       <c r="AE37" s="49">
-        <f>+AE12/AD12-1</f>
+        <f t="shared" si="83"/>
         <v>5.8406356413166938E-2</v>
       </c>
       <c r="AF37" s="49">
-        <f>+AF12/AE12-1</f>
+        <f t="shared" si="83"/>
         <v>-7.9754969671491205E-2</v>
       </c>
       <c r="AG37" s="49">
-        <f>+AG12/AF12-1</f>
+        <f t="shared" si="83"/>
         <v>0.21995879210523861</v>
       </c>
       <c r="AH37" s="42"/>
@@ -5177,47 +5178,47 @@
         <v>40</v>
       </c>
       <c r="G38" s="49">
-        <f t="shared" ref="G38:L38" si="83">+G13/C13-1</f>
+        <f t="shared" ref="G38:L38" si="86">+G13/C13-1</f>
         <v>0.1766423357664233</v>
       </c>
       <c r="H38" s="49">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0.16496350364963508</v>
       </c>
       <c r="I38" s="49">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0.21199442119944223</v>
       </c>
       <c r="J38" s="49">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0.20202020202020199</v>
       </c>
       <c r="K38" s="49">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>6.3275434243176276E-2</v>
       </c>
       <c r="L38" s="49">
-        <f t="shared" si="83"/>
+        <f t="shared" si="86"/>
         <v>0.16541353383458657</v>
       </c>
       <c r="M38" s="49">
-        <f>+M13/I13-1</f>
+        <f t="shared" si="85"/>
         <v>6.6743383199079354E-2</v>
       </c>
       <c r="N38" s="49">
-        <f>+N13/J13-1</f>
+        <f t="shared" si="85"/>
         <v>-0.17331932773109238</v>
       </c>
       <c r="O38" s="49">
-        <f>+O13/K13-1</f>
+        <f t="shared" si="85"/>
         <v>0.17152858809801641</v>
       </c>
       <c r="P38" s="49">
-        <f>+P13/L13-1</f>
+        <f t="shared" si="85"/>
         <v>-0.15268817204301077</v>
       </c>
       <c r="Q38" s="49">
-        <f>+Q13/M13-1</f>
+        <f t="shared" si="85"/>
         <v>-0.17907227615965493</v>
       </c>
       <c r="R38" s="39"/>
@@ -5254,23 +5255,23 @@
         <v>41</v>
       </c>
       <c r="G39" s="50">
-        <f t="shared" ref="G39:K39" si="84">+G14/C14-1</f>
+        <f t="shared" ref="G39:K39" si="87">+G14/C14-1</f>
         <v>-6.1642881312075737E-2</v>
       </c>
       <c r="H39" s="50">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>-0.3046877888276831</v>
       </c>
       <c r="I39" s="50">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>-1.5302691601693841E-2</v>
       </c>
       <c r="J39" s="50">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>-2.1075126192844684E-2</v>
       </c>
       <c r="K39" s="50">
-        <f t="shared" si="84"/>
+        <f t="shared" si="87"/>
         <v>8.7010011878499771E-2</v>
       </c>
       <c r="L39" s="50">
@@ -5278,39 +5279,39 @@
         <v>0.56530639372590707</v>
       </c>
       <c r="M39" s="50">
-        <f t="shared" ref="M39:O39" si="85">+M14/I14-1</f>
+        <f t="shared" ref="M39:O39" si="88">+M14/I14-1</f>
         <v>0.14455251841051298</v>
       </c>
       <c r="N39" s="50">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0.13084798072942139</v>
       </c>
       <c r="O39" s="50">
-        <f t="shared" si="85"/>
+        <f t="shared" si="88"/>
         <v>0.10556921515825635</v>
       </c>
       <c r="P39" s="50">
-        <f t="shared" ref="P39" si="86">+P14/L14-1</f>
+        <f t="shared" ref="P39" si="89">+P14/L14-1</f>
         <v>-2.8787853054569434E-2</v>
       </c>
       <c r="Q39" s="50">
-        <f t="shared" ref="Q39" si="87">+Q14/M14-1</f>
+        <f t="shared" ref="Q39" si="90">+Q14/M14-1</f>
         <v>-5.3085643332849486E-2</v>
       </c>
       <c r="R39" s="39">
-        <f t="shared" ref="R39" si="88">+R14/N14-1</f>
+        <f t="shared" ref="R39" si="91">+R14/N14-1</f>
         <v>9.1886553218327061E-2</v>
       </c>
       <c r="AD39" s="50">
-        <f t="shared" ref="AD39:AF39" si="89">+AD14/AC14-1</f>
+        <f t="shared" ref="AD39:AF39" si="92">+AD14/AC14-1</f>
         <v>-7.413633908816919E-2</v>
       </c>
       <c r="AE39" s="50">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>4.9957192989058541E-3</v>
       </c>
       <c r="AF39" s="50">
-        <f t="shared" si="89"/>
+        <f t="shared" si="92"/>
         <v>-0.10094362584486338</v>
       </c>
       <c r="AG39" s="50">
@@ -5318,39 +5319,39 @@
         <v>0.20903487125022102</v>
       </c>
       <c r="AH39" s="39">
-        <f t="shared" ref="AH39:AP39" si="90">+AH14/AG14-1</f>
+        <f t="shared" ref="AH39:AP39" si="93">+AH14/AG14-1</f>
         <v>2.5597814525500473E-2</v>
       </c>
       <c r="AI39" s="39">
-        <f t="shared" si="90"/>
+        <f>+AI14/AH14-1</f>
         <v>4.1326663331665792E-2</v>
       </c>
       <c r="AJ39" s="39">
-        <f t="shared" si="90"/>
+        <f>+AJ14/AI14-1</f>
         <v>5.3934450800629641E-2</v>
       </c>
       <c r="AK39" s="39">
-        <f t="shared" si="90"/>
+        <f>+AK14/AJ14-1</f>
         <v>7.4260720240910016E-2</v>
       </c>
       <c r="AL39" s="39">
-        <f t="shared" si="90"/>
+        <f>+AL14/AK14-1</f>
         <v>8.455120101137803E-2</v>
       </c>
       <c r="AM39" s="39">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>8.4798696650292493E-2</v>
       </c>
       <c r="AN39" s="39">
-        <f t="shared" si="90"/>
+        <f>+AN14/AM14-1</f>
         <v>8.5042884175862143E-2</v>
       </c>
       <c r="AO39" s="39">
-        <f t="shared" si="90"/>
+        <f>+AO14/AN14-1</f>
         <v>8.5283628091289421E-2</v>
       </c>
       <c r="AP39" s="39">
-        <f t="shared" si="90"/>
+        <f t="shared" si="93"/>
         <v>8.5520800370000982E-2</v>
       </c>
       <c r="AQ39" s="39">
@@ -5383,123 +5384,123 @@
         <v>0.4290121613821381</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" ref="D41:R41" si="91">+D22/D14</f>
+        <f t="shared" ref="D41:R41" si="94">+D22/D14</f>
         <v>0.43201227402122072</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.4504116460389293</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.43504292398953615</v>
       </c>
       <c r="G41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.37483030714406929</v>
       </c>
       <c r="H41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.2743852186627676</v>
       </c>
       <c r="I41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.48027906461674769</v>
       </c>
       <c r="J41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.41838232526628782</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.45997736408695317</v>
       </c>
       <c r="L41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.47116968698517292</v>
       </c>
       <c r="M41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.49515424185251483</v>
       </c>
       <c r="N41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.41330648516416757</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.42454462016379552</v>
       </c>
       <c r="P41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.29934946838276449</v>
       </c>
       <c r="Q41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.4706834011682362</v>
       </c>
       <c r="R41" s="5">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>0.41330648516416757</v>
       </c>
       <c r="AC41" s="5">
-        <f t="shared" ref="AC41:AQ41" si="92">+AC22/AC14</f>
+        <f t="shared" ref="AC41:AQ41" si="95">+AC22/AC14</f>
         <v>0.50010888312050317</v>
       </c>
       <c r="AD41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.51880686041151169</v>
       </c>
       <c r="AE41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.43681545000093613</v>
       </c>
       <c r="AF41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.3969533210466582</v>
       </c>
       <c r="AG41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.46013202485477694</v>
       </c>
       <c r="AH41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.40276551478737616</v>
       </c>
       <c r="AI41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.46216973537784167</v>
       </c>
       <c r="AJ41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.45884670307299136</v>
       </c>
       <c r="AK41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.45564100315594558</v>
       </c>
       <c r="AL41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.45266823549720253</v>
       </c>
       <c r="AM41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.44994513664712693</v>
       </c>
       <c r="AN41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.44745189934755941</v>
       </c>
       <c r="AO41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.4451702103978592</v>
       </c>
       <c r="AP41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.44308314342601957</v>
       </c>
       <c r="AQ41" s="5">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>0.44117505899487797</v>
       </c>
       <c r="AT41" s="1" t="s">
@@ -5507,7 +5508,7 @@
       </c>
       <c r="AU41" s="1">
         <f>+Main!J4</f>
-        <v>277.8</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="2:53">
@@ -5529,7 +5530,7 @@
       </c>
       <c r="AU42" s="6">
         <f>+AU40/AU41-1</f>
-        <v>3.7502091857323006E-2</v>
+        <v>4.8065749519870415E-2</v>
       </c>
     </row>
     <row r="43" spans="2:53">
@@ -5565,7 +5566,7 @@
       </c>
       <c r="Q44" s="1">
         <f>+Main!J6</f>
-        <v>203467.2738576</v>
+        <v>201416.4878</v>
       </c>
       <c r="AC44" s="1">
         <f>+AC28*AC43</f>
@@ -5616,47 +5617,47 @@
         <v>5</v>
       </c>
       <c r="J45" s="1">
-        <f>+J44+J48</f>
+        <f t="shared" ref="J45:O45" si="96">+J44+J48</f>
         <v>-32694.100000000002</v>
       </c>
       <c r="K45" s="1">
-        <f>+K44+K48</f>
+        <f t="shared" si="96"/>
         <v>-31492.399999999998</v>
       </c>
       <c r="L45" s="1">
-        <f>+L44+L48</f>
+        <f t="shared" si="96"/>
         <v>-31176.399999999998</v>
       </c>
       <c r="M45" s="1">
-        <f>+M44+M48</f>
+        <f t="shared" si="96"/>
         <v>-29650.799999999999</v>
       </c>
       <c r="N45" s="1">
-        <f>+N44+N48</f>
+        <f t="shared" si="96"/>
         <v>-29712.299999999996</v>
       </c>
       <c r="O45" s="1">
-        <f>+O44+O48</f>
+        <f t="shared" si="96"/>
         <v>157794.5</v>
       </c>
       <c r="Q45" s="1">
         <f>+Q44+Q48</f>
-        <v>176160.97385760001</v>
+        <v>174110.18780000001</v>
       </c>
       <c r="AC45" s="1">
-        <f t="shared" ref="AC45:AF45" si="93">+AC44+AC48</f>
+        <f t="shared" ref="AC45:AF45" si="97">+AC44+AC48</f>
         <v>140363.86000000002</v>
       </c>
       <c r="AD45" s="1">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>139498.992</v>
       </c>
       <c r="AE45" s="1">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>157684.25368020311</v>
       </c>
       <c r="AF45" s="1">
-        <f t="shared" si="93"/>
+        <f t="shared" si="97"/>
         <v>139912.89286846283</v>
       </c>
       <c r="AG45" s="1">
@@ -5687,7 +5688,7 @@
         <v>231.67424552599149</v>
       </c>
       <c r="AZ45" s="1">
-        <f t="shared" ref="AZ45:BA45" si="94">FV(AZ44,10,,-$AG$29)*$AT$44</f>
+        <f t="shared" ref="AZ45" si="98">FV(AZ44,10,,-$AG$29)*$AT$44</f>
         <v>210.13927420879025</v>
       </c>
     </row>
@@ -5734,7 +5735,7 @@
         <v>128</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" ref="J48" si="95">+J49+J54-J69-J71</f>
+        <f t="shared" ref="J48" si="99">+J49+J54-J69-J71</f>
         <v>-32694.100000000002</v>
       </c>
       <c r="K48" s="3">
@@ -5746,15 +5747,15 @@
         <v>-31176.399999999998</v>
       </c>
       <c r="M48" s="3">
-        <f t="shared" ref="M48:O48" si="96">+M49+M54-M69-M71</f>
+        <f t="shared" ref="M48:O48" si="100">+M49+M54-M69-M71</f>
         <v>-29650.799999999999</v>
       </c>
       <c r="N48" s="3">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>-29712.299999999996</v>
       </c>
       <c r="O48" s="3">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>-30475.9</v>
       </c>
       <c r="P48" s="3">
@@ -5762,11 +5763,11 @@
         <v>-29287.9</v>
       </c>
       <c r="Q48" s="3">
-        <f t="shared" ref="Q48:R48" si="97">+P48+Q27</f>
+        <f t="shared" ref="Q48:R48" si="101">+P48+Q27</f>
         <v>-27306.300000000003</v>
       </c>
       <c r="R48" s="3">
-        <f t="shared" si="97"/>
+        <f t="shared" si="101"/>
         <v>-25557.273535479311</v>
       </c>
       <c r="AF48" s="3">
@@ -5782,39 +5783,39 @@
         <v>-25557.273535479311</v>
       </c>
       <c r="AI48" s="3">
-        <f t="shared" ref="AI48:AP48" si="98">+AH48+AI27</f>
+        <f t="shared" ref="AI48:AP48" si="102">+AH48+AI27</f>
         <v>-18249.51371059454</v>
       </c>
       <c r="AJ48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>-10602.991064531465</v>
       </c>
       <c r="AK48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>-2446.0211749181872</v>
       </c>
       <c r="AL48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>6342.9115428965688</v>
       </c>
       <c r="AM48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>15819.779643913707</v>
       </c>
       <c r="AN48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>26045.608813957675</v>
       </c>
       <c r="AO48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>37086.942209522735</v>
       </c>
       <c r="AP48" s="3">
-        <f t="shared" si="98"/>
+        <f t="shared" si="102"/>
         <v>49016.347859827358</v>
       </c>
       <c r="AQ48" s="3">
-        <f t="shared" ref="AQ48" si="99">+AP48+AQ27</f>
+        <f t="shared" ref="AQ48" si="103">+AP48+AQ27</f>
         <v>61912.973137994282</v>
       </c>
       <c r="AT48" s="44" t="s">
@@ -5822,7 +5823,7 @@
       </c>
       <c r="AU48" s="6">
         <f>+AU47/AU41-1</f>
-        <v>-1.5818350818804672E-2</v>
+        <v>-5.797592208959701E-3</v>
       </c>
     </row>
     <row r="49" spans="2:46">
@@ -5947,35 +5948,35 @@
         <v>57</v>
       </c>
       <c r="J53" s="3">
-        <f t="shared" ref="J53:P53" si="100">+SUM(J49:J52)</f>
+        <f t="shared" ref="J53:P53" si="104">+SUM(J49:J52)</f>
         <v>6243.2</v>
       </c>
       <c r="K53" s="3">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>5467.9</v>
       </c>
       <c r="L53" s="3">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>5701.2</v>
       </c>
       <c r="M53" s="3">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>6795.9000000000005</v>
       </c>
       <c r="N53" s="3">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>7148.5000000000009</v>
       </c>
       <c r="O53" s="3">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>4656.3999999999996</v>
       </c>
       <c r="P53" s="3">
-        <f t="shared" si="100"/>
+        <f t="shared" si="104"/>
         <v>4919.3</v>
       </c>
       <c r="Q53" s="3">
-        <f t="shared" ref="Q53" si="101">+SUM(Q49:Q52)</f>
+        <f t="shared" ref="Q53" si="105">+SUM(Q49:Q52)</f>
         <v>5740.8</v>
       </c>
     </row>
@@ -6071,35 +6072,35 @@
         <v>61</v>
       </c>
       <c r="J57" s="3">
-        <f t="shared" ref="J57:P57" si="102">+SUM(J54:J56)</f>
+        <f t="shared" ref="J57:P57" si="106">+SUM(J54:J56)</f>
         <v>7597.7000000000007</v>
       </c>
       <c r="K57" s="3">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>7456</v>
       </c>
       <c r="L57" s="3">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>7864.4</v>
       </c>
       <c r="M57" s="3">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>7973.5</v>
       </c>
       <c r="N57" s="3">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>8433.2000000000007</v>
       </c>
       <c r="O57" s="3">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>8408</v>
       </c>
       <c r="P57" s="3">
-        <f t="shared" si="102"/>
+        <f t="shared" si="106"/>
         <v>8199.7999999999993</v>
       </c>
       <c r="Q57" s="3">
-        <f t="shared" ref="Q57" si="103">+SUM(Q54:Q56)</f>
+        <f t="shared" ref="Q57" si="107">+SUM(Q54:Q56)</f>
         <v>7869.7000000000007</v>
       </c>
     </row>
@@ -6166,35 +6167,35 @@
         <v>53</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" ref="J60:Q60" si="104">+J53+J57+SUM(J58:J59)</f>
+        <f t="shared" ref="J60:Q60" si="108">+J53+J57+SUM(J58:J59)</f>
         <v>52626.8</v>
       </c>
       <c r="K60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>51103.1</v>
       </c>
       <c r="L60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>51893.1</v>
       </c>
       <c r="M60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>52727</v>
       </c>
       <c r="N60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>53854.3</v>
       </c>
       <c r="O60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>50877.700000000004</v>
       </c>
       <c r="P60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>49247.799999999996</v>
       </c>
       <c r="Q60" s="3">
-        <f t="shared" si="104"/>
+        <f t="shared" si="108"/>
         <v>48501.599999999999</v>
       </c>
     </row>
@@ -6420,35 +6421,35 @@
         <v>64</v>
       </c>
       <c r="J70" s="3">
-        <f t="shared" ref="J70:P70" si="105">+SUM(J62:J69)</f>
+        <f t="shared" ref="J70:P70" si="109">+SUM(J62:J69)</f>
         <v>6181.2000000000007</v>
       </c>
       <c r="K70" s="3">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>4579.7999999999993</v>
       </c>
       <c r="L70" s="3">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>3934.7999999999997</v>
       </c>
       <c r="M70" s="3">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>5095.5999999999995</v>
       </c>
       <c r="N70" s="3">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>4020</v>
       </c>
       <c r="O70" s="3">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>4234.6000000000004</v>
       </c>
       <c r="P70" s="3">
-        <f t="shared" si="105"/>
+        <f t="shared" si="109"/>
         <v>3480.1</v>
       </c>
       <c r="Q70" s="3">
-        <f t="shared" ref="Q70" si="106">+SUM(Q62:Q69)</f>
+        <f t="shared" ref="Q70" si="110">+SUM(Q62:Q69)</f>
         <v>3486.0999999999995</v>
       </c>
     </row>
@@ -6631,35 +6632,35 @@
         <v>72</v>
       </c>
       <c r="J77" s="3">
-        <f t="shared" ref="J77:P77" si="107">SUM(J70:J76)</f>
+        <f t="shared" ref="J77:P77" si="111">SUM(J70:J76)</f>
         <v>60451.7</v>
       </c>
       <c r="K77" s="3">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>58338.600000000006</v>
       </c>
       <c r="L77" s="3">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>57701.1</v>
       </c>
       <c r="M77" s="3">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>58401.999999999993</v>
       </c>
       <c r="N77" s="3">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>58455.3</v>
       </c>
       <c r="O77" s="3">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>56868.5</v>
       </c>
       <c r="P77" s="3">
-        <f t="shared" si="107"/>
+        <f t="shared" si="111"/>
         <v>55617.599999999999</v>
       </c>
       <c r="Q77" s="3">
-        <f t="shared" ref="Q77" si="108">SUM(Q70:Q76)</f>
+        <f t="shared" ref="Q77" si="112">SUM(Q70:Q76)</f>
         <v>55067.799999999996</v>
       </c>
     </row>
@@ -6697,35 +6698,35 @@
         <v>74</v>
       </c>
       <c r="J79" s="3">
-        <f t="shared" ref="J79:P79" si="109">+J77+J78</f>
+        <f t="shared" ref="J79:P79" si="113">+J77+J78</f>
         <v>52626.799999999996</v>
       </c>
       <c r="K79" s="3">
-        <f t="shared" si="109"/>
+        <f t="shared" si="113"/>
         <v>51103.100000000006</v>
       </c>
       <c r="L79" s="3">
-        <f t="shared" si="109"/>
+        <f t="shared" si="113"/>
         <v>51893.1</v>
       </c>
       <c r="M79" s="3">
-        <f t="shared" si="109"/>
+        <f t="shared" si="113"/>
         <v>52726.999999999993</v>
       </c>
       <c r="N79" s="3">
-        <f t="shared" si="109"/>
+        <f t="shared" si="113"/>
         <v>53854.3</v>
       </c>
       <c r="O79" s="3">
-        <f t="shared" si="109"/>
+        <f t="shared" si="113"/>
         <v>50877.7</v>
       </c>
       <c r="P79" s="3">
-        <f t="shared" si="109"/>
+        <f t="shared" si="113"/>
         <v>49247.799999999996</v>
       </c>
       <c r="Q79" s="3">
-        <f t="shared" ref="Q79" si="110">+Q77+Q78</f>
+        <f t="shared" ref="Q79" si="114">+Q77+Q78</f>
         <v>48501.599999999999</v>
       </c>
     </row>
@@ -6734,35 +6735,35 @@
         <v>93</v>
       </c>
       <c r="J80" s="25" t="str">
-        <f t="shared" ref="J80:P80" si="111">IF(J60=J79,"True","False")</f>
+        <f t="shared" ref="J80:P80" si="115">IF(J60=J79,"True","False")</f>
         <v>True</v>
       </c>
       <c r="K80" s="25" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="115"/>
         <v>True</v>
       </c>
       <c r="L80" s="25" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="115"/>
         <v>True</v>
       </c>
       <c r="M80" s="25" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="115"/>
         <v>True</v>
       </c>
       <c r="N80" s="25" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="115"/>
         <v>True</v>
       </c>
       <c r="O80" s="25" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="115"/>
         <v>True</v>
       </c>
       <c r="P80" s="25" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="115"/>
         <v>True</v>
       </c>
       <c r="Q80" s="25" t="str">
-        <f t="shared" ref="Q80" si="112">IF(Q60=Q79,"True","False")</f>
+        <f t="shared" ref="Q80" si="116">IF(Q60=Q79,"True","False")</f>
         <v>True</v>
       </c>
     </row>
@@ -7031,7 +7032,7 @@
     <row r="110" spans="2:33">
       <c r="O110" s="5">
         <f>+O109/Main!J9</f>
-        <v>2.9419311204556847E-2</v>
+        <v>2.9677745898421704E-2</v>
       </c>
     </row>
     <row r="114" spans="2:16">

</xml_diff>